<commit_message>
add rank brand of workat module 3
</commit_message>
<xml_diff>
--- a/Результаты по модулям.xlsx
+++ b/Результаты по модулям.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Desktop/Project/Skillbox/DS/AnalystJunior/module_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3B2E3D-F356-6F47-A9CF-3B1D50D87F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA542A9B-8D2D-694F-8C7E-288D6A0CC94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="20700" windowHeight="13700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Данные (модуль 2)" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7888" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7926" uniqueCount="85">
   <si>
     <t>Year</t>
   </si>
@@ -247,18 +247,54 @@
   <si>
     <t>Green-Рынок дек.2022/дек.2021</t>
   </si>
+  <si>
+    <t>name Brand</t>
+  </si>
+  <si>
+    <t>2020, млн.руб.</t>
+  </si>
+  <si>
+    <t>Rank2020</t>
+  </si>
+  <si>
+    <t>Share2020, %</t>
+  </si>
+  <si>
+    <t>2021, млн.руб.</t>
+  </si>
+  <si>
+    <t>Rank2021</t>
+  </si>
+  <si>
+    <t>Share2021, %</t>
+  </si>
+  <si>
+    <t>2022, млн.руб.</t>
+  </si>
+  <si>
+    <t>Rank2022</t>
+  </si>
+  <si>
+    <t>Share2022, %</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -275,7 +311,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -298,13 +334,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -82859,31 +82913,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -82896,8 +82955,8 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -82910,8 +82969,8 @@
         <v>-15.51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -82924,8 +82983,8 @@
         <v>-19.62</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -82938,8 +82997,8 @@
         <v>4.04</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -82952,8 +83011,8 @@
         <v>-6.36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -82966,8 +83025,8 @@
         <v>-7.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -82980,8 +83039,8 @@
         <v>-8.24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -82994,8 +83053,8 @@
         <v>-9.1499999999999986</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -83006,6 +83065,820 @@
       </c>
       <c r="D10">
         <v>-12.12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>496393.39746399998</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>66.650000000000006</v>
+      </c>
+      <c r="F17">
+        <v>522684.06106500002</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>65.92</v>
+      </c>
+      <c r="I17">
+        <v>500728.413849</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>60.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>137428.510446</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>18.45</v>
+      </c>
+      <c r="F18">
+        <v>163431.952433</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>20.61</v>
+      </c>
+      <c r="I18">
+        <v>221366.50213899999</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>26.83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>37160.190296000001</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>4.99</v>
+      </c>
+      <c r="F19">
+        <v>31878.142958</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="I19">
+        <v>31060.392489999998</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>5797.2830029999996</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>0.78</v>
+      </c>
+      <c r="F20">
+        <v>14061.567713</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>1.77</v>
+      </c>
+      <c r="I20">
+        <v>15712.971507</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>1878.9583239999999</v>
+      </c>
+      <c r="D21">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>0.25</v>
+      </c>
+      <c r="F21">
+        <v>2601.1356249999999</v>
+      </c>
+      <c r="G21">
+        <v>11</v>
+      </c>
+      <c r="H21">
+        <v>0.33</v>
+      </c>
+      <c r="I21">
+        <v>15480.62132</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22">
+        <v>5688.7062910000004</v>
+      </c>
+      <c r="D22">
+        <v>7</v>
+      </c>
+      <c r="E22">
+        <v>0.76</v>
+      </c>
+      <c r="F22">
+        <v>5259.9316070000004</v>
+      </c>
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>0.66</v>
+      </c>
+      <c r="I22">
+        <v>5900.4470929999998</v>
+      </c>
+      <c r="J22">
+        <v>7</v>
+      </c>
+      <c r="K22">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>14288.243952999999</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>1.92</v>
+      </c>
+      <c r="F23">
+        <v>6131.2491629999986</v>
+      </c>
+      <c r="G23">
+        <v>8</v>
+      </c>
+      <c r="H23">
+        <v>0.77</v>
+      </c>
+      <c r="I23">
+        <v>4388.8159610000002</v>
+      </c>
+      <c r="J23">
+        <v>9</v>
+      </c>
+      <c r="K23">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>2575.655467</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>0.35</v>
+      </c>
+      <c r="F24">
+        <v>2454.9113860000002</v>
+      </c>
+      <c r="G24">
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <v>0.31</v>
+      </c>
+      <c r="I24">
+        <v>1456.9284279999999</v>
+      </c>
+      <c r="J24">
+        <v>12</v>
+      </c>
+      <c r="K24">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <v>2027.173865</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>0.27</v>
+      </c>
+      <c r="F25">
+        <v>974.82457099999999</v>
+      </c>
+      <c r="G25">
+        <v>14</v>
+      </c>
+      <c r="H25">
+        <v>0.12</v>
+      </c>
+      <c r="I25">
+        <v>1197.3275759999999</v>
+      </c>
+      <c r="J25">
+        <v>13</v>
+      </c>
+      <c r="K25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>27664.037851000001</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>3.71</v>
+      </c>
+      <c r="F26">
+        <v>9420.7652269999999</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>1.19</v>
+      </c>
+      <c r="I26">
+        <v>428.72448700000001</v>
+      </c>
+      <c r="J26">
+        <v>17</v>
+      </c>
+      <c r="K26">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27">
+        <v>1243.01133</v>
+      </c>
+      <c r="D27">
+        <v>13</v>
+      </c>
+      <c r="E27">
+        <v>0.17</v>
+      </c>
+      <c r="F27">
+        <v>469.84472599999998</v>
+      </c>
+      <c r="G27">
+        <v>18</v>
+      </c>
+      <c r="H27">
+        <v>0.06</v>
+      </c>
+      <c r="I27">
+        <v>426.93183699999997</v>
+      </c>
+      <c r="J27">
+        <v>18</v>
+      </c>
+      <c r="K27">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28">
+        <v>376.243831</v>
+      </c>
+      <c r="D28">
+        <v>20</v>
+      </c>
+      <c r="E28">
+        <v>0.05</v>
+      </c>
+      <c r="F28">
+        <v>230.07754499999999</v>
+      </c>
+      <c r="G28">
+        <v>21</v>
+      </c>
+      <c r="H28">
+        <v>0.03</v>
+      </c>
+      <c r="I28">
+        <v>182.54365300000001</v>
+      </c>
+      <c r="J28">
+        <v>21</v>
+      </c>
+      <c r="K28">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29">
+        <v>443.09228300000001</v>
+      </c>
+      <c r="D29">
+        <v>17</v>
+      </c>
+      <c r="E29">
+        <v>0.06</v>
+      </c>
+      <c r="F29">
+        <v>141.74029100000001</v>
+      </c>
+      <c r="G29">
+        <v>23</v>
+      </c>
+      <c r="H29">
+        <v>0.02</v>
+      </c>
+      <c r="I29">
+        <v>67.815393</v>
+      </c>
+      <c r="J29">
+        <v>23</v>
+      </c>
+      <c r="K29">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>5471.2506380000004</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>0.73</v>
+      </c>
+      <c r="F30">
+        <v>642.82823699999994</v>
+      </c>
+      <c r="G30">
+        <v>16</v>
+      </c>
+      <c r="H30">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31">
+        <v>2904.4837649999999</v>
+      </c>
+      <c r="D31">
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32">
+        <v>851.23158899999999</v>
+      </c>
+      <c r="D32">
+        <v>14</v>
+      </c>
+      <c r="E32">
+        <v>0.11</v>
+      </c>
+      <c r="F32">
+        <v>913.03659999999991</v>
+      </c>
+      <c r="G32">
+        <v>15</v>
+      </c>
+      <c r="H32">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33">
+        <v>617.31757500000003</v>
+      </c>
+      <c r="D33">
+        <v>15</v>
+      </c>
+      <c r="E33">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34">
+        <v>492.13755400000002</v>
+      </c>
+      <c r="D34">
+        <v>16</v>
+      </c>
+      <c r="E34">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F34">
+        <v>68.459952999999999</v>
+      </c>
+      <c r="G34">
+        <v>25</v>
+      </c>
+      <c r="H34">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35">
+        <v>407.43288000000001</v>
+      </c>
+      <c r="D35">
+        <v>18</v>
+      </c>
+      <c r="E35">
+        <v>0.05</v>
+      </c>
+      <c r="F35">
+        <v>6901.2733859999998</v>
+      </c>
+      <c r="G35">
+        <v>7</v>
+      </c>
+      <c r="H35">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>397.94978600000002</v>
+      </c>
+      <c r="D36">
+        <v>19</v>
+      </c>
+      <c r="E36">
+        <v>0.05</v>
+      </c>
+      <c r="F36">
+        <v>476.89962500000001</v>
+      </c>
+      <c r="G36">
+        <v>17</v>
+      </c>
+      <c r="H36">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37">
+        <v>206.92770899999999</v>
+      </c>
+      <c r="D37">
+        <v>21</v>
+      </c>
+      <c r="E37">
+        <v>0.03</v>
+      </c>
+      <c r="F37">
+        <v>272.22758299999998</v>
+      </c>
+      <c r="G37">
+        <v>19</v>
+      </c>
+      <c r="H37">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38">
+        <v>164.01495299999999</v>
+      </c>
+      <c r="D38">
+        <v>22</v>
+      </c>
+      <c r="E38">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39">
+        <v>90.161597999999998</v>
+      </c>
+      <c r="D39">
+        <v>23</v>
+      </c>
+      <c r="E39">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>23</v>
+      </c>
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40">
+        <v>86.020452000000006</v>
+      </c>
+      <c r="D40">
+        <v>24</v>
+      </c>
+      <c r="E40">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>58.388658999999997</v>
+      </c>
+      <c r="D41">
+        <v>25</v>
+      </c>
+      <c r="E41">
+        <v>0.01</v>
+      </c>
+      <c r="F41">
+        <v>65.683319999999995</v>
+      </c>
+      <c r="G41">
+        <v>26</v>
+      </c>
+      <c r="H41">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42">
+        <v>42.527850000000001</v>
+      </c>
+      <c r="D42">
+        <v>26</v>
+      </c>
+      <c r="E42">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>26</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <v>35.519098999999997</v>
+      </c>
+      <c r="D43">
+        <v>27</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>27</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44">
+        <v>30.692945999999999</v>
+      </c>
+      <c r="D44">
+        <v>28</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>50.093305000000001</v>
+      </c>
+      <c r="G44">
+        <v>27</v>
+      </c>
+      <c r="H44">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>